<commit_message>
tests results files added to temp directory + tests scripts on tests directory
</commit_message>
<xml_diff>
--- a/temp/tests_results_scenario_1.xlsx
+++ b/temp/tests_results_scenario_1.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -355,15 +355,15 @@
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
     <col width="7" customWidth="1" min="6" max="6"/>
-    <col width="21" customWidth="1" min="7" max="7"/>
+    <col width="7" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="21" customWidth="1" min="9" max="9"/>
     <col width="21" customWidth="1" min="10" max="10"/>
-    <col width="7" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -379,47 +379,47 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>classifier</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>fp</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>fn</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>tp</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>tn</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>avg_misclassification</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>sensitivity</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>specificity</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>classifier</t>
         </is>
       </c>
     </row>
@@ -431,31 +431,47 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1740</v>
-      </c>
-      <c r="D2" t="n">
-        <v>157</v>
-      </c>
-      <c r="E2" t="n">
-        <v>251</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5543</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.7589492631844138</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.2410507368155863</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.5877959360956647</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.7693619681315389</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1668</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>199</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>219</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>5605</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.75855952</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.24144048</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0.58458493</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.7689767</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -466,31 +482,47 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1721</v>
-      </c>
-      <c r="D3" t="n">
-        <v>169</v>
-      </c>
-      <c r="E3" t="n">
-        <v>267</v>
-      </c>
-      <c r="F3" t="n">
-        <v>5534</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.7586896246620896</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.2413103753379104</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.5865468225670142</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.7690849093812121</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1717</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>258</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>5515</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.75873237</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.24126763</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.5878099</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.76910174</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -501,31 +533,47 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>52</v>
-      </c>
-      <c r="D4" t="n">
-        <v>106</v>
-      </c>
-      <c r="E4" t="n">
-        <v>318</v>
-      </c>
-      <c r="F4" t="n">
-        <v>7215</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.9775938716654115</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.02240612833458859</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.738128953082224</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.9920487493369928</v>
-      </c>
-      <c r="K4" t="n">
         <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>338</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>7179</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.97733392</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.02266608</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0.73743386</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.9918187</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -536,31 +584,47 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>56</v>
-      </c>
-      <c r="D5" t="n">
-        <v>100</v>
-      </c>
-      <c r="E5" t="n">
-        <v>338</v>
-      </c>
-      <c r="F5" t="n">
-        <v>7197</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.977247146055391</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.02275285394460896</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.7335505485531183</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.9919591760193661</v>
-      </c>
-      <c r="K5" t="n">
         <v>2</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>109</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>327</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>7195</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.9771171</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.0228829</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.73282699</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.99186615</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -571,31 +635,47 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>2524</v>
-      </c>
-      <c r="D6" t="n">
-        <v>81</v>
-      </c>
-      <c r="E6" t="n">
-        <v>235</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2920</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.544817924807293</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.455182075192707</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.7356828317280363</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.5335632240110116</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2536</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>212</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2931</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0.54516547</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.45483453</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.73352379</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.53399036</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -606,31 +686,47 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>2538</v>
-      </c>
-      <c r="D7" t="n">
-        <v>80</v>
-      </c>
-      <c r="E7" t="n">
-        <v>247</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2895</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.5445289948536455</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.4554710051463545</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.7337087766148368</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.5333306818496671</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2432</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>232</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2993</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0.54614908</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.45385092</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.73271437</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.53517151</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -641,31 +737,47 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>120</v>
-      </c>
-      <c r="D8" t="n">
-        <v>103</v>
-      </c>
-      <c r="E8" t="n">
-        <v>229</v>
-      </c>
-      <c r="F8" t="n">
-        <v>5308</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.95856745670119</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.04143254329881</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.6733220416512725</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.9754256445397682</v>
-      </c>
-      <c r="K8" t="n">
         <v>2</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>133</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>206</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>5311</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0.95862498</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.04137502</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>0.67383394</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.97548259</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -676,31 +788,455 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>133</v>
-      </c>
-      <c r="D9" t="n">
-        <v>113</v>
-      </c>
-      <c r="E9" t="n">
-        <v>189</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5325</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.9585094758336709</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.04149052416632915</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.6733948518776215</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.975298819656124</v>
-      </c>
-      <c r="K9" t="n">
         <v>2</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>209</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>5320</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>0.95897248</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.04102752</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>0.67264793</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.97597035</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>996</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>298</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>4725</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0.82603928</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.17396072</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0.84387037</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.82488712</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1032</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>294</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>4689</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0.82620389</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.17379611</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.84418239</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.82517262</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>284</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>5741</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0.99275159</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.00724841</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0.88639461</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.99889659</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>311</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>5724</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0.99242209</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.00757791</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0.88175663</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.99878085</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1775</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>166</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>3433</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0.63473054</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.36526946</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>0.50333231</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.64244228</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1860</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>3342</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0.63418617</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.36581383</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>0.50539849</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0.64161045</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>223</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>5131</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0.96733805</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0.03266195</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>0.73227023</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.98093364</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>5147</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0.96721708</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.03278292</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.72660043</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0.98092555</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final adjustment on all scripts related to testing
</commit_message>
<xml_diff>
--- a/temp/tests_results_scenario_1.xlsx
+++ b/temp/tests_results_scenario_1.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,42 +435,42 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1668</t>
+          <t>3982</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>107</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>219</t>
+          <t>313</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>5605</t>
+          <t>3289</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.75855952</t>
+          <t>0.45856824</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.24144048</t>
+          <t>0.54143176</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.58458493</t>
+          <t>0.70899284</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.7689767</t>
+          <t>0.4434608</t>
         </is>
       </c>
     </row>
@@ -486,42 +486,42 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1717</t>
+          <t>4041</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>108</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>301</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5515</t>
+          <t>3241</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.75873237</t>
+          <t>0.46008476</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.24126763</t>
+          <t>0.53991524</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.5878099</t>
+          <t>0.69853779</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.76910174</t>
+          <t>0.4457809</t>
         </is>
       </c>
     </row>
@@ -537,42 +537,42 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>86</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>58</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>338</t>
+          <t>379</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>7179</t>
+          <t>7168</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.97733392</t>
+          <t>0.98257773</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.02266608</t>
+          <t>0.01742227</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.73743386</t>
+          <t>0.85802523</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.9918187</t>
+          <t>0.99012041</t>
         </is>
       </c>
     </row>
@@ -588,654 +588,1878 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>76</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>73</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>327</t>
+          <t>399</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>7195</t>
+          <t>7143</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.9771171</t>
+          <t>0.98257769</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.0228829</t>
+          <t>0.01742231</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.73282699</t>
+          <t>0.86048941</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.99186615</t>
+          <t>0.98998244</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2536</t>
+          <t>48</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>81</t>
+          <t>77</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>212</t>
+          <t>363</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2931</t>
+          <t>7203</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.54516547</t>
+          <t>0.98587154</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.45483453</t>
+          <t>0.01412846</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.73352379</t>
+          <t>0.85003243</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.53399036</t>
+          <t>0.99407187</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2432</t>
+          <t>41</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>67</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>401</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2993</t>
+          <t>7182</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.54614908</t>
+          <t>0.98604493</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.45385092</t>
+          <t>0.01395507</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.73271437</t>
+          <t>0.84617475</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.53517151</t>
+          <t>0.99443887</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>533</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>410</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>5311</t>
+          <t>6741</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.95862498</t>
+          <t>0.93070118</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>0.04137502</t>
+          <t>0.06929882</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.67383394</t>
+          <t>0.97958009</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.97548259</t>
+          <t>0.92775865</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>530</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>407</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>5320</t>
+          <t>6746</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.95897248</t>
+          <t>0.93048451</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.04102752</t>
+          <t>0.06951549</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.67264793</t>
+          <t>0.97652406</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.97597035</t>
+          <t>0.92771226</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>996</t>
+          <t>41</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>56</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>298</t>
+          <t>399</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>4725</t>
+          <t>7195</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.82603928</t>
+          <t>0.98773505</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.17396072</t>
+          <t>0.01226495</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.84387037</t>
+          <t>0.87193196</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.82488712</t>
+          <t>0.99471462</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1032</t>
+          <t>33</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>51</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>294</t>
+          <t>389</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>4689</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.82620389</t>
+          <t>0.98717175</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.17379611</t>
+          <t>0.01282825</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.84418239</t>
+          <t>0.86424561</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.82517262</t>
+          <t>0.99457664</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1189</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>343</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>5741</t>
+          <t>4227</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.99275159</t>
+          <t>0.79283593</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.00724841</t>
+          <t>0.20716407</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0.88639461</t>
+          <t>0.98936043</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0.99889659</t>
+          <t>0.78118313</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1176</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>311</t>
+          <t>337</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5724</t>
+          <t>4245</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0.99242209</t>
+          <t>0.79277834</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.00757791</t>
+          <t>0.20722166</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>0.88175663</t>
+          <t>0.98956202</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>0.99878085</t>
+          <t>0.78112402</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1775</t>
+          <t>139</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>98</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>203</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3433</t>
+          <t>5320</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.63473054</t>
+          <t>0.95602094</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.36526946</t>
+          <t>0.04397906</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.50333231</t>
+          <t>0.66890342</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>0.64244228</t>
+          <t>0.97302313</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1860</t>
+          <t>132</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>113</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>233</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>3342</t>
+          <t>5282</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.63418617</t>
+          <t>0.95561602</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.36581383</t>
+          <t>0.04438398</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.50539849</t>
+          <t>0.66936562</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>0.64161045</t>
+          <t>0.97254635</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>36</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>34</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>223</t>
+          <t>270</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>5131</t>
+          <t>5420</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.96733805</t>
+          <t>0.98645916</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.03266195</t>
+          <t>0.01354084</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.73227023</t>
+          <t>0.88242457</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>0.98093364</t>
+          <t>0.99264485</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>282</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>5413</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0.98755864</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.01244136</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>0.89665599</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0.99295095</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
         <v>4</v>
       </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="n">
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>369</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>239</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>5066</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0.92349952</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.07650048</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0.7333192</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0.93478686</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>2</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>86</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>187</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>5147</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>0.96721708</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>0.03278292</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>0.72660043</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>0.98092555</t>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>4</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>328</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>238</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>5111</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0.92407856</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0.07592144</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0.73487026</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>0.93527561</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>174</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>5394</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0.96296526</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0.03703474</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0.46140549</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0.99264716</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>180</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>138</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>5402</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0.96290722</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0.03709278</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0.46465117</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0.99239998</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>955</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>280</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>4766</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0.8228543</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0.1771457</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0.83788428</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0.82206371</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>965</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>291</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>4757</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>0.82214064</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0.17785936</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>0.83369679</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0.82147879</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>264</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>5726</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0.98830376</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0.01169624</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>0.82758431</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0.99756069</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>283</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>5715</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0.98824899</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0.01175101</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>0.8278555</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0.99755997</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>3</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>265</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>5719</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0.9867113</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0.0132887</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>0.81585633</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>0.99657493</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>258</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>5726</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>0.98627202</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0.01372798</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>0.81154424</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0.99634113</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>3</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>595</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>307</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>5156</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0.90077443</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0.09922557</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>0.96962081</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>0.89679521</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>4</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>578</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>320</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>5165</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0.90159809</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0.09840191</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>0.97584741</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>0.89731627</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>5</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>295</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>5753</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0.99588157</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>0.00411843</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>0.94535597</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>0.99883908</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>5</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>319</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>5724</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>0.99538738</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>0.00461262</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>0.9390441</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>0.99860642</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>1057</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>297</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>4143</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>0.81249622</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>0.18750378</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>0.9388064</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>0.805186</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>997</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>279</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>4216</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>0.81219379</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>0.18780621</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>0.94001387</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>0.80481609</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>4</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>212</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>5082</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>0.96092663</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>0.03907337</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>0.67303596</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>0.97754659</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>5110</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>0.96044275</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>0.03955725</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>0.66782497</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>0.97735352</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>4</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>3</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>275</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>5143</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>0.98633037</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>0.01366963</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>0.88485438</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>0.99218835</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>4</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>3</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>260</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>5173</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>0.98639085</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>0.01360915</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>0.88121672</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>0.99245277</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>4</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>898</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>288</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>4299</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>0.82658925</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>0.17341075</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>0.91637382</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>0.82144964</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>4</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>4</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>974</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>269</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>4248</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>0.82695216</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>0.17304784</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>0.91449129</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>0.82190408</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>5</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>158</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>5216</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>0.97326559</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>0.02673441</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>0.59843551</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>0.99481865</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" t="n">
+        <v>5</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>136</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>5174</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>0.9736285</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>0.0263715</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>0.6117754</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>0.99456261</t>
         </is>
       </c>
     </row>

</xml_diff>